<commit_message>
updates all raw files with files from 3-6-2023
</commit_message>
<xml_diff>
--- a/data-raw/LFR_ReleaseFish_Raw.xlsx
+++ b/data-raw/LFR_ReleaseFish_Raw.xlsx
@@ -10,7 +10,7 @@
     <sheet sheetId="1" r:id="rId1" name="LFR_RST_ReleaseFish_EDI_Query"/>
   </sheets>
   <definedNames>
-    <definedName name="LFR_RST_ReleaseFish_EDI_Query">'LFR_RST_ReleaseFish_EDI_Query'!$A$1:$D$1</definedName>
+    <definedName name="LFR_RST_ReleaseFish_EDI_Query">'LFR_RST_ReleaseFish_EDI_Query'!$A$1:$D$3</definedName>
   </definedNames>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
@@ -343,7 +343,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -373,6 +373,28 @@
         </is>
       </c>
     </row>
+    <row outlineLevel="0" r="2">
+      <c r="A2" s="0">
+        <v>12</v>
+      </c>
+      <c r="B2" s="0">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0">
+        <v>263</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="3">
+      <c r="A3" s="0">
+        <v>12</v>
+      </c>
+      <c r="B3" s="0">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0">
+        <v>262</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>